<commit_message>
Commit Huy Le's documentation
</commit_message>
<xml_diff>
--- a/documentation/TaskTracking.xlsx
+++ b/documentation/TaskTracking.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26215"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28908"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bi/Google Drive/My Files/MUM/Courses/WAA/Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanhhuyle/Documents/Git/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,6 +18,9 @@
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -557,8 +560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="H52" sqref="H52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -624,8 +627,7 @@
         <v>13.5</v>
       </c>
       <c r="H4" s="1">
-        <f>SUM(H5:H20)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K4" s="1">
         <f>SUM(K5:K20)</f>
@@ -644,7 +646,7 @@
         <v>0.5</v>
       </c>
       <c r="H5" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5" s="2">
         <v>0</v>
@@ -661,7 +663,7 @@
         <v>2</v>
       </c>
       <c r="H6" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6" s="2">
         <v>0</v>
@@ -712,7 +714,7 @@
         <v>2</v>
       </c>
       <c r="H9" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K9" s="2">
         <v>0</v>
@@ -729,7 +731,7 @@
         <v>2</v>
       </c>
       <c r="H10" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K10" s="2">
         <v>0</v>
@@ -749,7 +751,7 @@
         <v>0.5</v>
       </c>
       <c r="H12" s="2">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="K12" s="2">
         <v>0</v>
@@ -766,7 +768,7 @@
         <v>0.5</v>
       </c>
       <c r="H13" s="2">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="K13" s="2">
         <v>0</v>
@@ -783,7 +785,7 @@
         <v>0.5</v>
       </c>
       <c r="H14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K14" s="2">
         <v>0</v>
@@ -834,7 +836,7 @@
         <v>0.5</v>
       </c>
       <c r="H17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K17" s="2">
         <v>0</v>
@@ -887,7 +889,7 @@
       </c>
       <c r="H21" s="8">
         <f>SUM(H22:H28)</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="K21" s="8">
         <f>SUM(K22:K28)</f>
@@ -905,6 +907,9 @@
       <c r="D22" s="2">
         <v>2</v>
       </c>
+      <c r="H22" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
@@ -913,6 +918,9 @@
       <c r="D23" s="2">
         <v>1</v>
       </c>
+      <c r="H23" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
@@ -921,6 +929,9 @@
       <c r="D24" s="2">
         <v>1</v>
       </c>
+      <c r="H24" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
@@ -929,6 +940,9 @@
       <c r="D25" s="2">
         <v>1</v>
       </c>
+      <c r="H25" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
@@ -937,6 +951,9 @@
       <c r="D26" s="2">
         <v>1</v>
       </c>
+      <c r="H26" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
@@ -945,6 +962,9 @@
       <c r="D27" s="2">
         <v>4</v>
       </c>
+      <c r="H27" s="2">
+        <v>4</v>
+      </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="N28" t="s">
@@ -960,8 +980,7 @@
         <v>3</v>
       </c>
       <c r="H29" s="5">
-        <f>SUM(H30:H33)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K29" s="5">
         <f>SUM(K30:K33)</f>
@@ -979,6 +998,9 @@
       <c r="D30" s="2">
         <v>1</v>
       </c>
+      <c r="H30" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
@@ -987,12 +1009,18 @@
       <c r="D31" s="2">
         <v>1</v>
       </c>
+      <c r="H31" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>35</v>
       </c>
       <c r="D32" s="2">
+        <v>1</v>
+      </c>
+      <c r="H32" s="2">
         <v>1</v>
       </c>
     </row>
@@ -1062,8 +1090,7 @@
         <v>3</v>
       </c>
       <c r="H40" s="5">
-        <f>SUM(H41:H44)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K40" s="5">
         <f>SUM(K41:K44)</f>
@@ -1089,6 +1116,9 @@
       <c r="D42" s="2">
         <v>1</v>
       </c>
+      <c r="H42">
+        <v>2</v>
+      </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
@@ -1097,6 +1127,9 @@
       <c r="D43" s="2">
         <v>1</v>
       </c>
+      <c r="H43">
+        <v>1</v>
+      </c>
     </row>
     <row r="45" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="8" t="s">
@@ -1133,8 +1166,7 @@
         <v>1</v>
       </c>
       <c r="H48" s="5">
-        <f>SUM(H49:H50)</f>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="K48" s="5">
         <f>SUM(K49:K50)</f>
@@ -1159,8 +1191,7 @@
         <v>2</v>
       </c>
       <c r="H51" s="5">
-        <f>SUM(H52:H53)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K51" s="5">
         <f>SUM(K52:K53)</f>
@@ -1185,8 +1216,7 @@
         <v>2</v>
       </c>
       <c r="H54" s="5">
-        <f>SUM(H55:H56)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K54" s="5">
         <f>SUM(K55:K56)</f>
@@ -1211,8 +1241,7 @@
         <v>2</v>
       </c>
       <c r="H57" s="5">
-        <f>SUM(H58:H61)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K57" s="5">
         <f>SUM(K58:K61)</f>
@@ -1233,20 +1262,17 @@
         <v>44</v>
       </c>
       <c r="D62" s="6">
-        <f>SUM(63:66)</f>
         <v>20</v>
       </c>
       <c r="H62" s="5">
-        <f>SUM(63:66)</f>
         <v>20</v>
       </c>
       <c r="K62" s="5">
-        <f>SUM(63:66)</f>
         <v>20</v>
       </c>
       <c r="N62" s="5">
         <f>SUM(63:66)</f>
-        <v>20</v>
+        <v>40</v>
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.2">
@@ -1256,6 +1282,9 @@
       <c r="D63" s="2">
         <v>4</v>
       </c>
+      <c r="H63">
+        <v>4</v>
+      </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
@@ -1264,6 +1293,9 @@
       <c r="D64" s="2">
         <v>8</v>
       </c>
+      <c r="H64">
+        <v>8</v>
+      </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
@@ -1272,6 +1304,9 @@
       <c r="D65" s="2">
         <v>8</v>
       </c>
+      <c r="H65">
+        <v>8</v>
+      </c>
     </row>
     <row r="67" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="8" t="s">
@@ -1281,9 +1316,9 @@
         <f>SUM(D4,D21,D29,D34,D40,D45,D48,D51,D5, D57, D62, D54)</f>
         <v>64</v>
       </c>
-      <c r="H67" s="5">
-        <f>SUM(H4,H21,H29,H34,H40,H45,H48,H51,H54)</f>
-        <v>0</v>
+      <c r="H67" s="6">
+        <f>SUM(H4,H21,H29,H34,H40,H45,H48,H51,H5, H57, H62, H54)</f>
+        <v>60.5</v>
       </c>
       <c r="K67" s="5">
         <f>SUM(K4,K21,K29,K34,K40,K45,K48,K51,K54)</f>

</xml_diff>